<commit_message>
function and output from work on SS
</commit_message>
<xml_diff>
--- a/DataObjects/specieslist_KSnotes_10.4.xlsx
+++ b/DataObjects/specieslist_KSnotes_10.4.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/Data/Regen_RProj/DataObjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8B12A3-58A6-DB4F-A59E-D70CBA9E1486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C8C720-0914-1E47-9038-25610FBA6EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21220" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27580" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SmallSeedling" sheetId="1" r:id="rId1"/>
-    <sheet name="LargeSeedling" sheetId="2" r:id="rId2"/>
-    <sheet name="Sapling" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="LargeSeedling" sheetId="2" r:id="rId3"/>
+    <sheet name="Sapling" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="160">
   <si>
     <t>Latin_Name</t>
   </si>
@@ -378,9 +379,6 @@
     <t>ROPS, FRAL, RHCA, ELUM</t>
   </si>
   <si>
-    <t>ACPE, FRAM, SAHU, FAGR, MASP, ACNE, CRSP</t>
-  </si>
-  <si>
     <t>again, could group tree oaks starting here</t>
   </si>
   <si>
@@ -424,6 +422,87 @@
   </si>
   <si>
     <t>BELE, BEPO, BESP</t>
+  </si>
+  <si>
+    <t>REDUCE TO 8 CATEGORIES</t>
+  </si>
+  <si>
+    <t>Shrub Oaks</t>
+  </si>
+  <si>
+    <t>QUIL, QUPR</t>
+  </si>
+  <si>
+    <t>Tree Oak</t>
+  </si>
+  <si>
+    <t>QUCO, QUAL, QUVE, QURU</t>
+  </si>
+  <si>
+    <t>PRSE, PRVI, PRPE, PRSP</t>
+  </si>
+  <si>
+    <t>HARDWOOD</t>
+  </si>
+  <si>
+    <t>SOFTWOOD</t>
+  </si>
+  <si>
+    <t>PIST, JUCO</t>
+  </si>
+  <si>
+    <t>INVASIVE</t>
+  </si>
+  <si>
+    <t>Is this category useful?</t>
+  </si>
+  <si>
+    <t>QUCO, QUAL, QUVE, QURU, QUPA</t>
+  </si>
+  <si>
+    <t>PRSE, PRVI, PRPE</t>
+  </si>
+  <si>
+    <t>ACPE, FRAM, SAHU, FAGR, MASP, ACNE, CRSP, ACPE, FRAM, SAHU, FAGR, MASP, ACNE, CRSP</t>
+  </si>
+  <si>
+    <t>SAAL, AMPS, BELE, BEPO, BENI, PODE, POGR, POTR, ACPE, FRAM, SAHU, FAGR, MASP, ACNE, CRSP</t>
+  </si>
+  <si>
+    <t>PIST, ABBA</t>
+  </si>
+  <si>
+    <t>FRAL, ROPS, RHCA, ELUM</t>
+  </si>
+  <si>
+    <t>AMPS, BELE, BEPO, BESP, PODE, POGR, POTR, MASP, NYSY, ACPE, CASP, CRSP, FAGR, FRAM</t>
+  </si>
+  <si>
+    <t>Tree Oaks</t>
+  </si>
+  <si>
+    <t>QUCO, QUAL, QUVE, QURU, QUPR, QUST</t>
+  </si>
+  <si>
+    <t>PRSE, FRPE, POGR, PODE, SAAL, AMSP, FAGR, NYSY, PRVI, ACNE, ACPE, MOSP, POTR, PRSP</t>
+  </si>
+  <si>
+    <t>Small Seedling Categories</t>
+  </si>
+  <si>
+    <t>Large Seedling Categories</t>
+  </si>
+  <si>
+    <t>Sapling Categories</t>
+  </si>
+  <si>
+    <t>AMPS, BELE, BEPO, BESP, PODE, POGR, POTR, MASP, NYSY, ACPE, CASP, CRSP, FAGR, FRAM, FRAL, ROPS, RHCA</t>
+  </si>
+  <si>
+    <t>SAAL, AMPS, BELE, BEPO, BENI, PODE, POGR, POTR, ACPE, FRAM, SAHU, FAGR, MASP, ACNE, CRSP, FRAL, ROPS, RHCA, ELUM</t>
+  </si>
+  <si>
+    <t>PRSE, FRPE, POGR, PODE, SAAL, AMSP, FAGR, NYSY, PRVI, ACNE, ACPE, MOSP, POTR, PRSP, FRAL, ROPS, RHCA, ELUM</t>
   </si>
 </sst>
 </file>
@@ -803,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -817,9 +896,11 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="9" max="9" width="62" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,8 +920,14 @@
         <v>83</v>
       </c>
       <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -860,8 +947,16 @@
         <v>84</v>
       </c>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -881,8 +976,14 @@
         <v>85</v>
       </c>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -902,8 +1003,14 @@
         <v>86</v>
       </c>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -923,8 +1030,14 @@
         <v>91</v>
       </c>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -944,8 +1057,16 @@
         <v>87</v>
       </c>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -965,8 +1086,12 @@
         <v>88</v>
       </c>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -986,8 +1111,16 @@
         <v>95</v>
       </c>
       <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1009,8 +1142,16 @@
       <c r="H9" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1032,8 +1173,16 @@
       <c r="H10" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
@@ -1053,8 +1202,18 @@
         <v>94</v>
       </c>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1074,8 +1233,12 @@
         <v>111</v>
       </c>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1093,8 +1256,12 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1112,8 +1279,12 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1133,8 +1304,12 @@
         <v>96</v>
       </c>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -1156,8 +1331,12 @@
       <c r="H16" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -1179,8 +1358,12 @@
       <c r="H17" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1200,10 +1383,14 @@
         <v>101</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1225,8 +1412,12 @@
       <c r="H19" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1244,8 +1435,12 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1263,8 +1458,12 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -1284,8 +1483,12 @@
         <v>104</v>
       </c>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -1307,8 +1510,12 @@
       <c r="H23" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
@@ -1330,8 +1537,12 @@
       <c r="H24" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -1353,8 +1564,12 @@
       <c r="H25" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1373,7 +1588,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
@@ -1392,7 +1607,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +1626,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -1430,7 +1645,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +1664,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1683,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1551,11 +1766,196 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659A1DAD-F094-1148-BDE3-3A5B9565023A}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:G26">
+    <sortCondition ref="A22:A26"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I2" sqref="I2:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1564,9 +1964,11 @@
     <col min="3" max="3" width="25.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="46" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -1586,8 +1988,14 @@
         <v>83</v>
       </c>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>70</v>
       </c>
@@ -1607,8 +2015,16 @@
         <v>84</v>
       </c>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
@@ -1628,8 +2044,16 @@
         <v>91</v>
       </c>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -1649,8 +2073,14 @@
         <v>88</v>
       </c>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
@@ -1670,8 +2100,16 @@
         <v>85</v>
       </c>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
@@ -1691,8 +2129,16 @@
         <v>86</v>
       </c>
       <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>66</v>
       </c>
@@ -1712,10 +2158,16 @@
         <v>92</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -1735,10 +2187,18 @@
         <v>89</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>74</v>
       </c>
@@ -1758,8 +2218,16 @@
         <v>87</v>
       </c>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>51</v>
       </c>
@@ -1779,8 +2247,18 @@
         <v>112</v>
       </c>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>78</v>
       </c>
@@ -1801,7 +2279,7 @@
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
@@ -1822,7 +2300,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -1843,7 +2321,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
@@ -1862,7 +2340,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>63</v>
       </c>
@@ -1883,7 +2361,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>62</v>
       </c>
@@ -1906,7 +2384,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
@@ -1929,7 +2407,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>76</v>
       </c>
@@ -1952,7 +2430,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
@@ -1974,8 +2452,12 @@
       <c r="H19" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>64</v>
       </c>
@@ -1993,8 +2475,12 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
@@ -2014,8 +2500,12 @@
         <v>104</v>
       </c>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
@@ -2037,8 +2527,12 @@
       <c r="H22" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -2058,10 +2552,14 @@
         <v>105</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2081,10 +2579,14 @@
         <v>107</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
@@ -2100,8 +2602,12 @@
       <c r="E25" s="2">
         <v>2.8169014084507</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>58</v>
       </c>
@@ -2117,8 +2623,12 @@
       <c r="E26" s="2">
         <v>2.8169014084507</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>75</v>
       </c>
@@ -2135,7 +2645,7 @@
         <v>2.8169014084507</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
@@ -2152,7 +2662,7 @@
         <v>1.8779342723004699</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
@@ -2169,7 +2679,7 @@
         <v>1.8779342723004699</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
@@ -2186,7 +2696,7 @@
         <v>1.8779342723004699</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>71</v>
       </c>
@@ -2203,7 +2713,7 @@
         <v>1.8779342723004699</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -2297,12 +2807,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2310,9 +2820,12 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -2332,8 +2845,14 @@
         <v>83</v>
       </c>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -2353,8 +2872,14 @@
         <v>85</v>
       </c>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>70</v>
       </c>
@@ -2374,8 +2899,16 @@
         <v>84</v>
       </c>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>60</v>
       </c>
@@ -2395,8 +2928,14 @@
         <v>87</v>
       </c>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -2416,8 +2955,16 @@
         <v>88</v>
       </c>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -2434,11 +2981,17 @@
         <v>23.661971830985902</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
@@ -2458,8 +3011,14 @@
         <v>86</v>
       </c>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>68</v>
       </c>
@@ -2479,8 +3038,16 @@
         <v>92</v>
       </c>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
@@ -2500,10 +3067,18 @@
         <v>91</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
@@ -2523,8 +3098,18 @@
         <v>94</v>
       </c>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>74</v>
       </c>
@@ -2543,7 +3128,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>72</v>
       </c>
@@ -2564,7 +3149,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>57</v>
       </c>
@@ -2584,10 +3169,10 @@
         <v>99</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -2607,10 +3192,10 @@
         <v>102</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -2627,13 +3212,13 @@
         <v>1.12676056338028</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>78</v>
       </c>
@@ -2652,7 +3237,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -2673,7 +3258,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -2690,13 +3275,13 @@
         <v>0.75117370892018798</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>80</v>
       </c>
@@ -2713,13 +3298,13 @@
         <v>0.75117370892018798</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -2736,13 +3321,13 @@
         <v>0.75117370892018798</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -2758,8 +3343,12 @@
       <c r="E21" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
@@ -2775,8 +3364,12 @@
       <c r="E22" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -2792,8 +3385,12 @@
       <c r="E23" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
@@ -2809,8 +3406,12 @@
       <c r="E24" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>79</v>
       </c>
@@ -2826,8 +3427,12 @@
       <c r="E25" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>64</v>
       </c>
@@ -2843,8 +3448,12 @@
       <c r="E26" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>81</v>
       </c>
@@ -2860,8 +3469,12 @@
       <c r="E27" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>73</v>
       </c>
@@ -2877,8 +3490,12 @@
       <c r="E28" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>82</v>
       </c>
@@ -2894,8 +3511,14 @@
       <c r="E29" s="2">
         <v>0.37558685446009399</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>75</v>
       </c>
@@ -2912,7 +3535,7 @@
         <v>0.37558685446009399</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>

</xml_diff>